<commit_message>
Added My hours to the burndown chart
</commit_message>
<xml_diff>
--- a/burndownchart.xlsx
+++ b/burndownchart.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\trophyHoardGame\Trophy-Hoard\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C63005A6-762E-4F6C-8E8B-D9FBBDC7C62C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Current Iteration" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Burndown Chart" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Current Iteration" sheetId="1" r:id="rId1"/>
+    <sheet name="Burndown Chart" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -21,12 +26,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author> </author>
+    <author/>
   </authors>
   <commentList>
-    <comment ref="G4" authorId="0">
+    <comment ref="G4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -60,147 +65,140 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
-    <t xml:space="preserve">Iteration Number:</t>
+    <t>Iteration Number:</t>
   </si>
   <si>
     <t xml:space="preserve">Expected Total effort: </t>
   </si>
   <si>
-    <t xml:space="preserve">Days In Sprint:</t>
+    <t>Days In Sprint:</t>
   </si>
   <si>
-    <t xml:space="preserve">Burndown Chart</t>
+    <t>Burndown Chart</t>
   </si>
   <si>
-    <t xml:space="preserve">User Stories</t>
+    <t>User Stories</t>
   </si>
   <si>
-    <t xml:space="preserve">Days (Points Completed)</t>
+    <t>Days (Points Completed)</t>
   </si>
   <si>
-    <t xml:space="preserve">Remaining</t>
+    <t>Remaining</t>
   </si>
   <si>
-    <t xml:space="preserve">Product Backlog Items</t>
+    <t>Product Backlog Items</t>
   </si>
   <si>
-    <t xml:space="preserve">Beginning Balance</t>
+    <t>Beginning Balance</t>
   </si>
   <si>
-    <t xml:space="preserve">Task Balance</t>
+    <t>Task Balance</t>
   </si>
   <si>
-    <t xml:space="preserve">Percentage Completed</t>
+    <t>Percentage Completed</t>
   </si>
   <si>
-    <t xml:space="preserve">Character Animations - Joseph</t>
+    <t>Character Animations - Joseph</t>
   </si>
   <si>
-    <t xml:space="preserve">Character Models - Joseph</t>
+    <t>Character Models - Joseph</t>
   </si>
   <si>
-    <t xml:space="preserve">Shield Powerup Implementation - Austin</t>
+    <t>Shield Powerup Implementation - Austin</t>
   </si>
   <si>
-    <t xml:space="preserve">Other Powerup - Austin</t>
+    <t>Other Powerup - Austin</t>
   </si>
   <si>
-    <t xml:space="preserve">Main Menus - Jerry</t>
+    <t>Main Menus - Jerry</t>
   </si>
   <si>
-    <t xml:space="preserve">In-game Menus - Braydon</t>
+    <t>In-game Menus - Braydon</t>
   </si>
   <si>
-    <t xml:space="preserve">Feature 7</t>
+    <t>Feature 7</t>
   </si>
   <si>
-    <t xml:space="preserve">Feature 8</t>
+    <t>Feature 8</t>
   </si>
   <si>
-    <t xml:space="preserve">Feature 9</t>
+    <t>Feature 9</t>
   </si>
   <si>
-    <t xml:space="preserve">Feature 10</t>
+    <t>Feature 10</t>
   </si>
   <si>
-    <t xml:space="preserve">Feature 11</t>
+    <t>Feature 11</t>
   </si>
   <si>
-    <t xml:space="preserve">Feature 12</t>
+    <t>Feature 12</t>
   </si>
   <si>
-    <t xml:space="preserve">Feature 13</t>
+    <t>Feature 13</t>
   </si>
   <si>
-    <t xml:space="preserve">Feature 14</t>
+    <t>Feature 14</t>
   </si>
   <si>
-    <t xml:space="preserve">Feature 15</t>
+    <t>Feature 15</t>
   </si>
   <si>
-    <t xml:space="preserve">Feature 16</t>
+    <t>Feature 16</t>
   </si>
   <si>
-    <t xml:space="preserve">Feature 17</t>
+    <t>Feature 17</t>
   </si>
   <si>
-    <t xml:space="preserve">Feature 18</t>
+    <t>Feature 18</t>
   </si>
   <si>
-    <t xml:space="preserve">Feature 19</t>
+    <t>Feature 19</t>
   </si>
   <si>
-    <t xml:space="preserve">Feature 20</t>
+    <t>Feature 20</t>
   </si>
   <si>
-    <t xml:space="preserve">Feature 21</t>
+    <t>Feature 21</t>
   </si>
   <si>
-    <t xml:space="preserve">Feature 22</t>
+    <t>Feature 22</t>
   </si>
   <si>
-    <t xml:space="preserve">Feature 23</t>
+    <t>Feature 23</t>
   </si>
   <si>
-    <t xml:space="preserve">Feature 24</t>
+    <t>Feature 24</t>
   </si>
   <si>
-    <t xml:space="preserve">Feature 25</t>
+    <t>Feature 25</t>
   </si>
   <si>
-    <t xml:space="preserve">Feature 26</t>
+    <t>Feature 26</t>
   </si>
   <si>
-    <t xml:space="preserve">Feature 27</t>
+    <t>Feature 27</t>
   </si>
   <si>
-    <t xml:space="preserve">Feature 28</t>
+    <t>Feature 28</t>
   </si>
   <si>
-    <t xml:space="preserve">Feature 29</t>
+    <t>Feature 29</t>
   </si>
   <si>
-    <t xml:space="preserve">Feature 30</t>
+    <t>Feature 30</t>
   </si>
   <si>
-    <t xml:space="preserve">Effort Remaining</t>
+    <t>Effort Remaining</t>
   </si>
   <si>
-    <t xml:space="preserve">Ideal Trend</t>
+    <t>Ideal Trend</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
-    <numFmt numFmtId="166" formatCode="0"/>
-    <numFmt numFmtId="167" formatCode="0.00%"/>
-    <numFmt numFmtId="168" formatCode="General"/>
-  </numFmts>
-  <fonts count="18">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -209,22 +207,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="30"/>
       <color rgb="FF203864"/>
       <name val="Malgun Gothic"/>
@@ -239,7 +222,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <color rgb="FF2F5597"/>
       <name val="Malgun Gothic"/>
@@ -247,7 +230,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF203864"/>
       <name val="Malgun Gothic"/>
@@ -255,7 +238,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF808080"/>
       <name val="Malgun Gothic"/>
@@ -263,7 +246,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF4472C4"/>
       <name val="Malgun Gothic"/>
@@ -271,7 +254,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Malgun Gothic"/>
@@ -284,45 +267,6 @@
       <name val="Tahoma"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="16"/>
-      <color rgb="FF595959"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF595959"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF595959"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="16"/>
-      <color rgb="FFF2F2F2"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FFD9D9D9"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="12"/>
-      <color rgb="FFD9D9D9"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="13">
@@ -400,14 +344,14 @@
     </fill>
   </fills>
   <borders count="31">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="dashed">
         <color rgb="FF203864"/>
       </left>
@@ -416,7 +360,7 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right style="thick">
         <color rgb="FF203864"/>
@@ -425,14 +369,22 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="medium"/>
-      <right style="medium"/>
-      <top style="medium"/>
-      <bottom style="medium"/>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -441,7 +393,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="dashed">
         <color rgb="FF203864"/>
       </left>
@@ -454,7 +406,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -465,7 +417,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="dashed">
         <color rgb="FF203864"/>
       </left>
@@ -480,7 +432,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="dashed">
         <color rgb="FF203864"/>
       </left>
@@ -491,7 +443,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="dashed">
         <color rgb="FF203864"/>
       </left>
@@ -506,7 +458,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right style="hair">
         <color rgb="FF203864"/>
@@ -519,7 +471,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="dashed">
         <color rgb="FF203864"/>
       </left>
@@ -532,7 +484,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top style="double">
@@ -543,7 +495,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="dashed">
         <color rgb="FF203864"/>
       </left>
@@ -556,7 +508,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right style="hair">
         <color rgb="FF203864"/>
@@ -569,7 +521,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="dashed">
         <color rgb="FF203864"/>
       </left>
@@ -582,7 +534,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top style="dashed">
@@ -593,7 +545,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right style="hair">
         <color rgb="FF203864"/>
@@ -604,7 +556,7 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="dashed">
         <color rgb="FF203864"/>
       </left>
@@ -615,7 +567,7 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top style="dashed">
@@ -624,7 +576,7 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="dashed">
         <color rgb="FF203864"/>
       </left>
@@ -639,7 +591,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right style="dashed">
         <color rgb="FF203864"/>
@@ -652,7 +604,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top style="medium">
@@ -663,7 +615,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="dashed">
         <color rgb="FF203864"/>
       </left>
@@ -678,7 +630,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="dashed">
         <color rgb="FF203864"/>
       </left>
@@ -693,7 +645,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="dashed">
         <color rgb="FF203864"/>
       </left>
@@ -704,7 +656,7 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right style="dashed">
         <color rgb="FF203864"/>
@@ -717,7 +669,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -728,7 +680,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="dashed">
         <color rgb="FF203864"/>
       </left>
@@ -743,7 +695,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="dashed">
         <color rgb="FF203864"/>
       </left>
@@ -754,7 +706,7 @@
       </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="dashed">
         <color rgb="FF203864"/>
       </left>
@@ -768,213 +720,137 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="43">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="14" fontId="5" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="6" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="6" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="6" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="1" fontId="2" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="6" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="1" fontId="2" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="4" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="7" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="4" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="1" fontId="2" fillId="7" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="1" fontId="2" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="4" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="7" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="4" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="1" fontId="2" fillId="7" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="1" fontId="2" fillId="4" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="4" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="7" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="4" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="1" fontId="7" fillId="10" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="10" fillId="8" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="10" fillId="9" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="10" fillId="10" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="10" fillId="11" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="10" fillId="12" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="29" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="30" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -1033,15 +909,33 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF2F5597"/>
       <rgbColor rgb="FF262626"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
+  <c:style val="2"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1050,7 +944,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="1" sz="1600" spc="117" strike="noStrike">
+              <a:defRPr sz="1600" b="1" strike="noStrike" spc="117">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
@@ -1058,7 +952,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr b="1" sz="1600" spc="117" strike="noStrike">
+              <a:rPr lang="en-US" sz="1600" b="1" strike="noStrike" spc="117">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
@@ -1079,6 +973,7 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
+      <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -1097,12 +992,9 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="4472c4"/>
-            </a:solidFill>
-            <a:ln cap="rnd" w="22320">
+            <a:ln w="22320" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="4472c4"/>
+                <a:srgbClr val="4472C4"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1112,23 +1004,31 @@
             <c:size val="6"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="4472c4"/>
+                <a:srgbClr val="4472C4"/>
               </a:solidFill>
             </c:spPr>
           </c:marker>
           <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:txPr>
               <a:bodyPr wrap="square"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
                     <a:latin typeface="Calibri"/>
                   </a:defRPr>
                 </a:pPr>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="r"/>
@@ -1137,8 +1037,9 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
             <c:separator>; </c:separator>
-            <c:showLeaderLines val="1"/>
+            <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="1"/>
@@ -1226,12 +1127,74 @@
                   <c:v>69</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>68</c:v>
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>#N/A</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6B86-420C-95CB-1CF94D4249B0}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1248,12 +1211,9 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="ed7d31"/>
-            </a:solidFill>
-            <a:ln cap="rnd" w="22320">
+            <a:ln w="22320" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="ed7d31"/>
+                <a:srgbClr val="ED7D31"/>
               </a:solidFill>
               <a:prstDash val="sysDot"/>
               <a:round/>
@@ -1264,23 +1224,31 @@
             <c:size val="6"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="ed7d31"/>
+                <a:srgbClr val="ED7D31"/>
               </a:solidFill>
             </c:spPr>
           </c:marker>
           <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:txPr>
               <a:bodyPr wrap="square"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
                     <a:latin typeface="Calibri"/>
                   </a:defRPr>
                 </a:pPr>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="r"/>
@@ -1289,8 +1257,9 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
             <c:separator>; </c:separator>
-            <c:showLeaderLines val="1"/>
+            <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="1"/>
@@ -1381,67 +1350,80 @@
                   <c:v>65.55</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>62.1</c:v>
+                  <c:v>62.099999999999994</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>58.65</c:v>
+                  <c:v>58.649999999999991</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>55.2</c:v>
+                  <c:v>55.199999999999989</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>51.75</c:v>
+                  <c:v>51.749999999999986</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>48.3</c:v>
+                  <c:v>48.299999999999983</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44.85</c:v>
+                  <c:v>44.84999999999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>41.4</c:v>
+                  <c:v>41.399999999999977</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>37.95</c:v>
+                  <c:v>37.949999999999974</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>34.5</c:v>
+                  <c:v>34.499999999999972</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>31.05</c:v>
+                  <c:v>31.049999999999972</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>27.6</c:v>
+                  <c:v>27.599999999999973</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>24.15</c:v>
+                  <c:v>24.149999999999974</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>20.7</c:v>
+                  <c:v>20.699999999999974</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>17.25</c:v>
+                  <c:v>17.249999999999975</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>13.8</c:v>
+                  <c:v>13.799999999999976</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>10.35</c:v>
+                  <c:v>10.349999999999977</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>6.89999999999998</c:v>
+                  <c:v>6.8999999999999764</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>3.44999999999998</c:v>
+                  <c:v>3.4499999999999762</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-2.39808173319034E-014</c:v>
+                  <c:v>-2.3980817331903381E-14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-6B86-420C-95CB-1CF94D4249B0}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:hiLowLines>
           <c:spPr>
             <a:ln w="0">
@@ -1450,6 +1432,7 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
+        <c:smooth val="0"/>
         <c:axId val="84044416"/>
         <c:axId val="17032541"/>
       </c:lineChart>
@@ -1464,7 +1447,7 @@
           <c:spPr>
             <a:ln w="9360">
               <a:solidFill>
-                <a:srgbClr val="d9d9d9"/>
+                <a:srgbClr val="D9D9D9"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1477,7 +1460,7 @@
         <c:spPr>
           <a:ln w="9360">
             <a:solidFill>
-              <a:srgbClr val="d9d9d9"/>
+              <a:srgbClr val="D9D9D9"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -1487,13 +1470,14 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="800" spc="117" strike="noStrike">
+              <a:defRPr sz="800" b="0" strike="noStrike" spc="117">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="17032541"/>
@@ -1517,7 +1501,7 @@
         <c:spPr>
           <a:ln w="9360">
             <a:solidFill>
-              <a:srgbClr val="d9d9d9"/>
+              <a:srgbClr val="D9D9D9"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -1527,13 +1511,14 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="84044416"/>
@@ -1561,22 +1546,24 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+            <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
               <a:solidFill>
                 <a:srgbClr val="595959"/>
               </a:solidFill>
               <a:latin typeface="Calibri"/>
             </a:defRPr>
           </a:pPr>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="1"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:srgbClr val="ffffff"/>
+      <a:srgbClr val="FFFFFF"/>
     </a:solidFill>
     <a:ln w="9360">
       <a:solidFill>
@@ -1585,13 +1572,20 @@
       <a:round/>
     </a:ln>
   </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
+  <c:style val="2"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1600,17 +1594,17 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="1" sz="1600" spc="97" strike="noStrike">
+              <a:defRPr sz="1600" b="1" strike="noStrike" spc="97">
                 <a:solidFill>
-                  <a:srgbClr val="f2f2f2"/>
+                  <a:srgbClr val="F2F2F2"/>
                 </a:solidFill>
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr b="1" sz="1600" spc="97" strike="noStrike">
+              <a:rPr sz="1600" b="1" strike="noStrike" spc="97">
                 <a:solidFill>
-                  <a:srgbClr val="f2f2f2"/>
+                  <a:srgbClr val="F2F2F2"/>
                 </a:solidFill>
                 <a:latin typeface="Calibri"/>
               </a:rPr>
@@ -1629,6 +1623,7 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
+      <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -1647,12 +1642,9 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="b4c7e7"/>
-            </a:solidFill>
-            <a:ln cap="rnd" w="34920">
+            <a:ln w="34920" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="b4c7e7"/>
+                <a:srgbClr val="B4C7E7"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1661,19 +1653,26 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:dLbls>
-            <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:txPr>
               <a:bodyPr wrap="square"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                  <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
-                      <a:srgbClr val="d9d9d9"/>
+                      <a:srgbClr val="D9D9D9"/>
                     </a:solidFill>
                     <a:latin typeface="Calibri"/>
                   </a:defRPr>
                 </a:pPr>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="t"/>
@@ -1682,8 +1681,9 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
             <c:separator>; </c:separator>
-            <c:showLeaderLines val="1"/>
+            <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="1"/>
@@ -1692,17 +1692,15 @@
           </c:dLbls>
           <c:trendline>
             <c:spPr>
-              <a:ln cap="rnd" w="19080">
+              <a:ln w="19080" cap="rnd">
                 <a:solidFill>
-                  <a:srgbClr val="4472c4"/>
+                  <a:srgbClr val="4472C4"/>
                 </a:solidFill>
                 <a:prstDash val="sysDash"/>
                 <a:round/>
               </a:ln>
             </c:spPr>
             <c:trendlineType val="linear"/>
-            <c:forward val="0"/>
-            <c:backward val="0"/>
             <c:dispRSqr val="0"/>
             <c:dispEq val="0"/>
           </c:trendline>
@@ -1787,12 +1785,74 @@
                   <c:v>69</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>68</c:v>
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>#N/A</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-FD30-425B-9C11-ED6E41907A92}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1809,14 +1869,9 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="bf9000">
-                <a:alpha val="31000"/>
-              </a:srgbClr>
-            </a:solidFill>
-            <a:ln cap="rnd" w="34920">
+            <a:ln w="34920" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="bf9000">
+                <a:srgbClr val="BF9000">
                   <a:alpha val="31000"/>
                 </a:srgbClr>
               </a:solidFill>
@@ -1828,19 +1883,26 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:dLbls>
-            <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:txPr>
               <a:bodyPr wrap="square"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                  <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
-                      <a:srgbClr val="d9d9d9"/>
+                      <a:srgbClr val="D9D9D9"/>
                     </a:solidFill>
                     <a:latin typeface="Calibri"/>
                   </a:defRPr>
                 </a:pPr>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="b"/>
@@ -1849,8 +1911,9 @@
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
             <c:separator>; </c:separator>
-            <c:showLeaderLines val="1"/>
+            <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="1"/>
@@ -1941,67 +2004,80 @@
                   <c:v>65.55</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>62.1</c:v>
+                  <c:v>62.099999999999994</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>58.65</c:v>
+                  <c:v>58.649999999999991</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>55.2</c:v>
+                  <c:v>55.199999999999989</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>51.75</c:v>
+                  <c:v>51.749999999999986</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>48.3</c:v>
+                  <c:v>48.299999999999983</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44.85</c:v>
+                  <c:v>44.84999999999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>41.4</c:v>
+                  <c:v>41.399999999999977</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>37.95</c:v>
+                  <c:v>37.949999999999974</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>34.5</c:v>
+                  <c:v>34.499999999999972</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>31.05</c:v>
+                  <c:v>31.049999999999972</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>27.6</c:v>
+                  <c:v>27.599999999999973</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>24.15</c:v>
+                  <c:v>24.149999999999974</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>20.7</c:v>
+                  <c:v>20.699999999999974</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>17.25</c:v>
+                  <c:v>17.249999999999975</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>13.8</c:v>
+                  <c:v>13.799999999999976</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>10.35</c:v>
+                  <c:v>10.349999999999977</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>6.89999999999998</c:v>
+                  <c:v>6.8999999999999764</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>3.44999999999998</c:v>
+                  <c:v>3.4499999999999762</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-2.39808173319034E-014</c:v>
+                  <c:v>-2.3980817331903381E-14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-FD30-425B-9C11-ED6E41907A92}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:hiLowLines>
           <c:spPr>
             <a:ln w="0">
@@ -2009,7 +2085,7 @@
             </a:ln>
           </c:spPr>
         </c:hiLowLines>
-        <c:marker val="0"/>
+        <c:smooth val="0"/>
         <c:axId val="98537599"/>
         <c:axId val="96963144"/>
       </c:lineChart>
@@ -2027,17 +2103,17 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="1" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+                  <a:defRPr lang="en-US" sz="1200" b="1" strike="noStrike" spc="-1">
                     <a:solidFill>
-                      <a:srgbClr val="d9d9d9"/>
+                      <a:srgbClr val="D9D9D9"/>
                     </a:solidFill>
                     <a:latin typeface="Calibri"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="1" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+                  <a:rPr lang="en-US" sz="1200" b="1" strike="noStrike" spc="-1">
                     <a:solidFill>
-                      <a:srgbClr val="d9d9d9"/>
+                      <a:srgbClr val="D9D9D9"/>
                     </a:solidFill>
                     <a:latin typeface="Calibri"/>
                   </a:rPr>
@@ -2061,7 +2137,7 @@
         <c:spPr>
           <a:ln w="9360">
             <a:solidFill>
-              <a:srgbClr val="f2f2f2">
+              <a:srgbClr val="F2F2F2">
                 <a:alpha val="10000"/>
               </a:srgbClr>
             </a:solidFill>
@@ -2073,13 +2149,14 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
-                  <a:srgbClr val="d9d9d9"/>
+                  <a:srgbClr val="D9D9D9"/>
                 </a:solidFill>
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="96963144"/>
@@ -2100,7 +2177,7 @@
           <c:spPr>
             <a:ln w="9360">
               <a:solidFill>
-                <a:srgbClr val="f2f2f2">
+                <a:srgbClr val="F2F2F2">
                   <a:alpha val="10000"/>
                 </a:srgbClr>
               </a:solidFill>
@@ -2115,17 +2192,17 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="1" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+                  <a:defRPr lang="en-US" sz="1200" b="1" strike="noStrike" spc="-1">
                     <a:solidFill>
-                      <a:srgbClr val="d9d9d9"/>
+                      <a:srgbClr val="D9D9D9"/>
                     </a:solidFill>
                     <a:latin typeface="Calibri"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="1" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+                  <a:rPr lang="en-US" sz="1200" b="1" strike="noStrike" spc="-1">
                     <a:solidFill>
-                      <a:srgbClr val="d9d9d9"/>
+                      <a:srgbClr val="D9D9D9"/>
                     </a:solidFill>
                     <a:latin typeface="Calibri"/>
                   </a:rPr>
@@ -2156,13 +2233,14 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+              <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
-                  <a:srgbClr val="d9d9d9"/>
+                  <a:srgbClr val="D9D9D9"/>
                 </a:solidFill>
                 <a:latin typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="98537599"/>
@@ -2190,18 +2268,20 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+            <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
               <a:solidFill>
-                <a:srgbClr val="d9d9d9"/>
+                <a:srgbClr val="D9D9D9"/>
               </a:solidFill>
               <a:latin typeface="Calibri"/>
             </a:defRPr>
           </a:pPr>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="1"/>
   </c:chart>
   <c:spPr>
     <a:gradFill>
@@ -2221,11 +2301,16 @@
       <a:noFill/>
     </a:ln>
   </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
@@ -2239,14 +2324,20 @@
       <xdr:row>4</xdr:row>
       <xdr:rowOff>1104480</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="0" name="Chart 2"/>
+        <xdr:cNvPr id="2" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8304840" y="66600"/>
-        <a:ext cx="7497720" cy="2047680"/>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2260,7 +2351,7 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -2274,14 +2365,20 @@
       <xdr:row>34</xdr:row>
       <xdr:rowOff>47160</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="1" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="237960" y="218880"/>
-        <a:ext cx="14054760" cy="6305400"/>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2294,267 +2391,558 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:X40"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:X39"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="7" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="C13" activeCellId="0" sqref="C13"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomRight" activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="70.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="3" style="0" width="5.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="18.14"/>
+    <col min="1" max="1" width="70.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="22" width="5.7109375" customWidth="1"/>
+    <col min="24" max="24" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="3"/>
-      <c r="X1" s="4"/>
+    <row r="1" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="U1" s="7"/>
+      <c r="V1" s="7"/>
+      <c r="W1" s="8"/>
+      <c r="X1" s="9"/>
     </row>
-    <row r="2" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
+    <row r="2" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
       <c r="C2" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
-      <c r="S2" s="2"/>
-      <c r="T2" s="2"/>
-      <c r="U2" s="2"/>
-      <c r="V2" s="2"/>
-      <c r="W2" s="3"/>
-      <c r="X2" s="4"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="7"/>
+      <c r="T2" s="7"/>
+      <c r="U2" s="7"/>
+      <c r="V2" s="7"/>
+      <c r="W2" s="8"/>
+      <c r="X2" s="9"/>
     </row>
-    <row r="3" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8"/>
+    <row r="3" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="11"/>
+      <c r="B3" s="11"/>
       <c r="C3" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
-      <c r="G3" s="6" t="n">
-        <f aca="false">B38</f>
+      <c r="G3" s="10">
+        <f>B38</f>
         <v>69</v>
       </c>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
-      <c r="S3" s="2"/>
-      <c r="T3" s="2"/>
-      <c r="U3" s="2"/>
-      <c r="V3" s="2"/>
-      <c r="W3" s="3"/>
-      <c r="X3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="7"/>
+      <c r="U3" s="7"/>
+      <c r="V3" s="7"/>
+      <c r="W3" s="8"/>
+      <c r="X3" s="9"/>
     </row>
-    <row r="4" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
+    <row r="4" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="11"/>
+      <c r="B4" s="11"/>
       <c r="C4" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
-      <c r="T4" s="2"/>
-      <c r="U4" s="2"/>
-      <c r="V4" s="2"/>
-      <c r="W4" s="3"/>
-      <c r="X4" s="4"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="7"/>
+      <c r="S4" s="7"/>
+      <c r="T4" s="7"/>
+      <c r="U4" s="7"/>
+      <c r="V4" s="7"/>
+      <c r="W4" s="8"/>
+      <c r="X4" s="9"/>
     </row>
-    <row r="5" customFormat="false" ht="97.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="8" t="s">
+    <row r="5" spans="1:24" ht="97.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
-      <c r="P5" s="2"/>
-      <c r="Q5" s="2"/>
-      <c r="R5" s="2"/>
-      <c r="S5" s="2"/>
-      <c r="T5" s="2"/>
-      <c r="U5" s="2"/>
-      <c r="V5" s="2"/>
-      <c r="W5" s="3"/>
-      <c r="X5" s="4"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="7"/>
+      <c r="S5" s="7"/>
+      <c r="T5" s="7"/>
+      <c r="U5" s="7"/>
+      <c r="V5" s="7"/>
+      <c r="W5" s="8"/>
+      <c r="X5" s="9"/>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="9" t="s">
+    <row r="6" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="10" t="s">
+      <c r="B6" s="3"/>
+      <c r="C6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10"/>
-      <c r="N6" s="10"/>
-      <c r="O6" s="10"/>
-      <c r="P6" s="10"/>
-      <c r="Q6" s="10"/>
-      <c r="R6" s="10"/>
-      <c r="S6" s="10"/>
-      <c r="T6" s="10"/>
-      <c r="U6" s="10"/>
-      <c r="V6" s="10"/>
-      <c r="W6" s="11" t="s">
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+      <c r="U6" s="2"/>
+      <c r="V6" s="2"/>
+      <c r="W6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="X6" s="11"/>
+      <c r="X6" s="1"/>
     </row>
-    <row r="7" customFormat="false" ht="45.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:24" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="12" t="n">
+      <c r="C7" s="12">
         <v>1</v>
       </c>
-      <c r="D7" s="12" t="n">
+      <c r="D7" s="12">
         <v>2</v>
       </c>
-      <c r="E7" s="12" t="n">
+      <c r="E7" s="12">
         <v>3</v>
       </c>
-      <c r="F7" s="12" t="n">
+      <c r="F7" s="12">
         <v>4</v>
       </c>
-      <c r="G7" s="12" t="n">
+      <c r="G7" s="12">
         <v>5</v>
       </c>
-      <c r="H7" s="12" t="n">
+      <c r="H7" s="12">
         <v>6</v>
       </c>
-      <c r="I7" s="12" t="n">
+      <c r="I7" s="12">
         <v>7</v>
       </c>
-      <c r="J7" s="12" t="n">
+      <c r="J7" s="12">
         <v>8</v>
       </c>
-      <c r="K7" s="12" t="n">
+      <c r="K7" s="12">
         <v>9</v>
       </c>
-      <c r="L7" s="12" t="n">
+      <c r="L7" s="12">
         <v>10</v>
       </c>
-      <c r="M7" s="12" t="n">
+      <c r="M7" s="12">
         <v>11</v>
       </c>
-      <c r="N7" s="12" t="n">
+      <c r="N7" s="12">
         <v>12</v>
       </c>
-      <c r="O7" s="12" t="n">
+      <c r="O7" s="12">
         <v>13</v>
       </c>
-      <c r="P7" s="12" t="n">
+      <c r="P7" s="12">
         <v>14</v>
       </c>
-      <c r="Q7" s="12" t="n">
+      <c r="Q7" s="12">
         <v>15</v>
       </c>
-      <c r="R7" s="12" t="n">
+      <c r="R7" s="12">
         <v>16</v>
       </c>
-      <c r="S7" s="12" t="n">
+      <c r="S7" s="12">
         <v>17</v>
       </c>
-      <c r="T7" s="12" t="n">
+      <c r="T7" s="12">
         <v>18</v>
       </c>
-      <c r="U7" s="12" t="n">
+      <c r="U7" s="12">
         <v>19</v>
       </c>
-      <c r="V7" s="12" t="n">
+      <c r="V7" s="12">
         <v>20</v>
       </c>
       <c r="W7" s="14" t="s">
@@ -2564,11 +2952,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="17" t="n">
+      <c r="B8" s="17">
         <v>20</v>
       </c>
       <c r="C8" s="18"/>
@@ -2591,20 +2979,20 @@
       <c r="T8" s="19"/>
       <c r="U8" s="18"/>
       <c r="V8" s="19"/>
-      <c r="W8" s="20" t="n">
-        <f aca="false">B8-SUM(C8:V8)</f>
+      <c r="W8" s="20">
+        <f t="shared" ref="W8:W37" si="0">B8-SUM(C8:V8)</f>
         <v>20</v>
       </c>
-      <c r="X8" s="21" t="n">
-        <f aca="false">IFERROR(1-(W8/B8),"")</f>
+      <c r="X8" s="21">
+        <f t="shared" ref="X8:X38" si="1">IFERROR(1-(W8/B8),"")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="23" t="n">
+      <c r="B9" s="23">
         <v>10</v>
       </c>
       <c r="C9" s="24"/>
@@ -2627,20 +3015,20 @@
       <c r="T9" s="25"/>
       <c r="U9" s="24"/>
       <c r="V9" s="25"/>
-      <c r="W9" s="26" t="n">
-        <f aca="false">B9-SUM(C9:V9)</f>
+      <c r="W9" s="26">
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="X9" s="21" t="n">
-        <f aca="false">IFERROR(1-(W9/B9),"")</f>
+      <c r="X9" s="21">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="23" t="n">
+      <c r="B10" s="23">
         <v>6</v>
       </c>
       <c r="C10" s="24"/>
@@ -2663,20 +3051,20 @@
       <c r="T10" s="25"/>
       <c r="U10" s="24"/>
       <c r="V10" s="25"/>
-      <c r="W10" s="26" t="n">
-        <f aca="false">B10-SUM(C10:V10)</f>
+      <c r="W10" s="26">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="X10" s="21" t="n">
-        <f aca="false">IFERROR(1-(W10/B10),"")</f>
+      <c r="X10" s="21">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="23" t="n">
+      <c r="B11" s="23">
         <v>6</v>
       </c>
       <c r="C11" s="24"/>
@@ -2699,128 +3087,156 @@
       <c r="T11" s="25"/>
       <c r="U11" s="24"/>
       <c r="V11" s="25"/>
-      <c r="W11" s="26" t="n">
-        <f aca="false">B11-SUM(C11:V11)</f>
+      <c r="W11" s="26">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="X11" s="21" t="n">
-        <f aca="false">IFERROR(1-(W11/B11),"")</f>
+      <c r="X11" s="21">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="23" t="n">
+      <c r="B12" s="23">
         <v>12</v>
       </c>
-      <c r="C12" s="24"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="25"/>
-      <c r="I12" s="24"/>
-      <c r="J12" s="25"/>
-      <c r="K12" s="24"/>
-      <c r="L12" s="25"/>
-      <c r="M12" s="24"/>
-      <c r="N12" s="25"/>
-      <c r="O12" s="24"/>
-      <c r="P12" s="25"/>
+      <c r="C12" s="24">
+        <v>2</v>
+      </c>
+      <c r="D12" s="25">
+        <v>1</v>
+      </c>
+      <c r="E12" s="24">
+        <v>0</v>
+      </c>
+      <c r="F12" s="25">
+        <v>0</v>
+      </c>
+      <c r="G12" s="24">
+        <v>2</v>
+      </c>
+      <c r="H12" s="25">
+        <v>3</v>
+      </c>
+      <c r="I12" s="24">
+        <v>0</v>
+      </c>
+      <c r="J12" s="25">
+        <v>1</v>
+      </c>
+      <c r="K12" s="24">
+        <v>-6</v>
+      </c>
+      <c r="L12" s="25">
+        <v>1</v>
+      </c>
+      <c r="M12" s="24">
+        <v>0</v>
+      </c>
+      <c r="N12" s="25">
+        <v>1</v>
+      </c>
+      <c r="O12" s="24">
+        <v>0</v>
+      </c>
+      <c r="P12" s="25">
+        <v>1</v>
+      </c>
       <c r="Q12" s="24"/>
       <c r="R12" s="25"/>
       <c r="S12" s="24"/>
       <c r="T12" s="25"/>
       <c r="U12" s="24"/>
       <c r="V12" s="25"/>
-      <c r="W12" s="26" t="n">
-        <f aca="false">B12-SUM(C12:V12)</f>
-        <v>12</v>
-      </c>
-      <c r="X12" s="21" t="n">
-        <f aca="false">IFERROR(1-(W12/B12),"")</f>
-        <v>0</v>
+      <c r="W12" s="26">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="X12" s="21">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="23" t="n">
+      <c r="B13" s="23">
         <v>15</v>
       </c>
-      <c r="C13" s="24" t="n">
+      <c r="C13" s="24">
         <v>1</v>
       </c>
-      <c r="D13" s="25" t="n">
+      <c r="D13" s="25">
         <v>0</v>
       </c>
-      <c r="E13" s="24" t="n">
+      <c r="E13" s="24">
         <v>0</v>
       </c>
-      <c r="F13" s="25" t="n">
+      <c r="F13" s="25">
         <v>0</v>
       </c>
-      <c r="G13" s="24" t="n">
+      <c r="G13" s="24">
         <v>1</v>
       </c>
-      <c r="H13" s="25" t="n">
+      <c r="H13" s="25">
         <v>2</v>
       </c>
-      <c r="I13" s="24" t="n">
+      <c r="I13" s="24">
         <v>0</v>
       </c>
-      <c r="J13" s="25" t="n">
+      <c r="J13" s="25">
         <v>0</v>
       </c>
-      <c r="K13" s="24" t="n">
+      <c r="K13" s="24">
         <v>2</v>
       </c>
-      <c r="L13" s="25" t="n">
+      <c r="L13" s="25">
         <v>0</v>
       </c>
-      <c r="M13" s="24" t="n">
+      <c r="M13" s="24">
         <v>2</v>
       </c>
-      <c r="N13" s="25" t="n">
+      <c r="N13" s="25">
         <v>0</v>
       </c>
-      <c r="O13" s="24" t="n">
+      <c r="O13" s="24">
         <v>-3</v>
       </c>
-      <c r="P13" s="25" t="n">
+      <c r="P13" s="25">
         <v>4</v>
       </c>
-      <c r="Q13" s="24" t="n">
+      <c r="Q13" s="24">
         <v>0</v>
       </c>
-      <c r="R13" s="25" t="n">
+      <c r="R13" s="25">
         <v>0</v>
       </c>
-      <c r="S13" s="24" t="n">
+      <c r="S13" s="24">
         <v>1</v>
       </c>
-      <c r="T13" s="25" t="n">
+      <c r="T13" s="25">
         <v>2</v>
       </c>
-      <c r="U13" s="24" t="n">
+      <c r="U13" s="24">
         <v>2</v>
       </c>
-      <c r="V13" s="25" t="n">
+      <c r="V13" s="25">
         <v>-6</v>
       </c>
-      <c r="W13" s="26" t="n">
-        <f aca="false">B13-SUM(C13:V13)</f>
+      <c r="W13" s="26">
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="X13" s="21" t="n">
-        <f aca="false">IFERROR(1-(W13/B13),"")</f>
-        <v>0.533333333333333</v>
+      <c r="X13" s="21">
+        <f t="shared" si="1"/>
+        <v>0.53333333333333333</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="22" t="s">
         <v>17</v>
       </c>
@@ -2845,16 +3261,16 @@
       <c r="T14" s="25"/>
       <c r="U14" s="24"/>
       <c r="V14" s="25"/>
-      <c r="W14" s="26" t="n">
-        <f aca="false">B14-SUM(C14:V14)</f>
+      <c r="W14" s="26">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="X14" s="21" t="str">
-        <f aca="false">IFERROR(1-(W14/B14),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="22" t="s">
         <v>18</v>
       </c>
@@ -2879,16 +3295,16 @@
       <c r="T15" s="25"/>
       <c r="U15" s="24"/>
       <c r="V15" s="25"/>
-      <c r="W15" s="26" t="n">
-        <f aca="false">B15-SUM(C15:V15)</f>
+      <c r="W15" s="26">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="X15" s="21" t="str">
-        <f aca="false">IFERROR(1-(W15/B15),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="22" t="s">
         <v>19</v>
       </c>
@@ -2913,16 +3329,16 @@
       <c r="T16" s="25"/>
       <c r="U16" s="24"/>
       <c r="V16" s="25"/>
-      <c r="W16" s="26" t="n">
-        <f aca="false">B16-SUM(C16:V16)</f>
+      <c r="W16" s="26">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="X16" s="21" t="str">
-        <f aca="false">IFERROR(1-(W16/B16),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="22" t="s">
         <v>20</v>
       </c>
@@ -2947,16 +3363,16 @@
       <c r="T17" s="25"/>
       <c r="U17" s="24"/>
       <c r="V17" s="25"/>
-      <c r="W17" s="26" t="n">
-        <f aca="false">B17-SUM(C17:V17)</f>
+      <c r="W17" s="26">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="X17" s="21" t="str">
-        <f aca="false">IFERROR(1-(W17/B17),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="22" t="s">
         <v>21</v>
       </c>
@@ -2981,16 +3397,16 @@
       <c r="T18" s="25"/>
       <c r="U18" s="24"/>
       <c r="V18" s="25"/>
-      <c r="W18" s="26" t="n">
-        <f aca="false">B18-SUM(C18:V18)</f>
+      <c r="W18" s="26">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="X18" s="21" t="str">
-        <f aca="false">IFERROR(1-(W18/B18),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="22" t="s">
         <v>22</v>
       </c>
@@ -3015,16 +3431,16 @@
       <c r="T19" s="25"/>
       <c r="U19" s="24"/>
       <c r="V19" s="25"/>
-      <c r="W19" s="26" t="n">
-        <f aca="false">B19-SUM(C19:V19)</f>
+      <c r="W19" s="26">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="X19" s="21" t="str">
-        <f aca="false">IFERROR(1-(W19/B19),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="22" t="s">
         <v>23</v>
       </c>
@@ -3049,16 +3465,16 @@
       <c r="T20" s="25"/>
       <c r="U20" s="24"/>
       <c r="V20" s="25"/>
-      <c r="W20" s="26" t="n">
-        <f aca="false">B20-SUM(C20:V20)</f>
+      <c r="W20" s="26">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="X20" s="21" t="str">
-        <f aca="false">IFERROR(1-(W20/B20),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="22" t="s">
         <v>24</v>
       </c>
@@ -3083,16 +3499,16 @@
       <c r="T21" s="25"/>
       <c r="U21" s="24"/>
       <c r="V21" s="25"/>
-      <c r="W21" s="26" t="n">
-        <f aca="false">B21-SUM(C21:V21)</f>
+      <c r="W21" s="26">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="X21" s="21" t="str">
-        <f aca="false">IFERROR(1-(W21/B21),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="22" t="s">
         <v>25</v>
       </c>
@@ -3117,16 +3533,16 @@
       <c r="T22" s="25"/>
       <c r="U22" s="24"/>
       <c r="V22" s="25"/>
-      <c r="W22" s="26" t="n">
-        <f aca="false">B22-SUM(C22:V22)</f>
+      <c r="W22" s="26">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="X22" s="21" t="str">
-        <f aca="false">IFERROR(1-(W22/B22),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="22" t="s">
         <v>26</v>
       </c>
@@ -3151,16 +3567,16 @@
       <c r="T23" s="25"/>
       <c r="U23" s="24"/>
       <c r="V23" s="25"/>
-      <c r="W23" s="26" t="n">
-        <f aca="false">B23-SUM(C23:V23)</f>
+      <c r="W23" s="26">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="X23" s="21" t="str">
-        <f aca="false">IFERROR(1-(W23/B23),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="22" t="s">
         <v>27</v>
       </c>
@@ -3185,16 +3601,16 @@
       <c r="T24" s="25"/>
       <c r="U24" s="24"/>
       <c r="V24" s="25"/>
-      <c r="W24" s="26" t="n">
-        <f aca="false">B24-SUM(C24:V24)</f>
+      <c r="W24" s="26">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="X24" s="21" t="str">
-        <f aca="false">IFERROR(1-(W24/B24),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="22" t="s">
         <v>28</v>
       </c>
@@ -3219,16 +3635,16 @@
       <c r="T25" s="25"/>
       <c r="U25" s="24"/>
       <c r="V25" s="25"/>
-      <c r="W25" s="26" t="n">
-        <f aca="false">B25-SUM(C25:V25)</f>
+      <c r="W25" s="26">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="X25" s="21" t="str">
-        <f aca="false">IFERROR(1-(W25/B25),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="22" t="s">
         <v>29</v>
       </c>
@@ -3253,16 +3669,16 @@
       <c r="T26" s="25"/>
       <c r="U26" s="24"/>
       <c r="V26" s="25"/>
-      <c r="W26" s="26" t="n">
-        <f aca="false">B26-SUM(C26:V26)</f>
+      <c r="W26" s="26">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="X26" s="21" t="str">
-        <f aca="false">IFERROR(1-(W26/B26),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="22" t="s">
         <v>30</v>
       </c>
@@ -3287,16 +3703,16 @@
       <c r="T27" s="25"/>
       <c r="U27" s="24"/>
       <c r="V27" s="25"/>
-      <c r="W27" s="26" t="n">
-        <f aca="false">B27-SUM(C27:V27)</f>
+      <c r="W27" s="26">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="X27" s="21" t="str">
-        <f aca="false">IFERROR(1-(W27/B27),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="22" t="s">
         <v>31</v>
       </c>
@@ -3321,16 +3737,16 @@
       <c r="T28" s="25"/>
       <c r="U28" s="24"/>
       <c r="V28" s="25"/>
-      <c r="W28" s="26" t="n">
-        <f aca="false">B28-SUM(C28:V28)</f>
+      <c r="W28" s="26">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="X28" s="21" t="str">
-        <f aca="false">IFERROR(1-(W28/B28),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="22" t="s">
         <v>32</v>
       </c>
@@ -3355,16 +3771,16 @@
       <c r="T29" s="25"/>
       <c r="U29" s="24"/>
       <c r="V29" s="25"/>
-      <c r="W29" s="26" t="n">
-        <f aca="false">B29-SUM(C29:V29)</f>
+      <c r="W29" s="26">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="X29" s="21" t="str">
-        <f aca="false">IFERROR(1-(W29/B29),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="22" t="s">
         <v>33</v>
       </c>
@@ -3389,16 +3805,16 @@
       <c r="T30" s="25"/>
       <c r="U30" s="24"/>
       <c r="V30" s="25"/>
-      <c r="W30" s="26" t="n">
-        <f aca="false">B30-SUM(C30:V30)</f>
+      <c r="W30" s="26">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="X30" s="21" t="str">
-        <f aca="false">IFERROR(1-(W30/B30),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="22" t="s">
         <v>34</v>
       </c>
@@ -3423,16 +3839,16 @@
       <c r="T31" s="25"/>
       <c r="U31" s="24"/>
       <c r="V31" s="25"/>
-      <c r="W31" s="26" t="n">
-        <f aca="false">B31-SUM(C31:V31)</f>
+      <c r="W31" s="26">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="X31" s="21" t="str">
-        <f aca="false">IFERROR(1-(W31/B31),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="22" t="s">
         <v>35</v>
       </c>
@@ -3457,16 +3873,16 @@
       <c r="T32" s="25"/>
       <c r="U32" s="24"/>
       <c r="V32" s="25"/>
-      <c r="W32" s="26" t="n">
-        <f aca="false">B32-SUM(C32:V32)</f>
+      <c r="W32" s="26">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="X32" s="21" t="str">
-        <f aca="false">IFERROR(1-(W32/B32),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="22" t="s">
         <v>36</v>
       </c>
@@ -3491,16 +3907,16 @@
       <c r="T33" s="25"/>
       <c r="U33" s="24"/>
       <c r="V33" s="25"/>
-      <c r="W33" s="26" t="n">
-        <f aca="false">B33-SUM(C33:V33)</f>
+      <c r="W33" s="26">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="X33" s="21" t="str">
-        <f aca="false">IFERROR(1-(W33/B33),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="22" t="s">
         <v>37</v>
       </c>
@@ -3525,16 +3941,16 @@
       <c r="T34" s="25"/>
       <c r="U34" s="24"/>
       <c r="V34" s="25"/>
-      <c r="W34" s="26" t="n">
-        <f aca="false">B34-SUM(C34:V34)</f>
+      <c r="W34" s="26">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="X34" s="21" t="str">
-        <f aca="false">IFERROR(1-(W34/B34),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="22" t="s">
         <v>38</v>
       </c>
@@ -3559,16 +3975,16 @@
       <c r="T35" s="25"/>
       <c r="U35" s="24"/>
       <c r="V35" s="25"/>
-      <c r="W35" s="26" t="n">
-        <f aca="false">B35-SUM(C35:V35)</f>
+      <c r="W35" s="26">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="X35" s="21" t="str">
-        <f aca="false">IFERROR(1-(W35/B35),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="22" t="s">
         <v>39</v>
       </c>
@@ -3593,16 +4009,16 @@
       <c r="T36" s="25"/>
       <c r="U36" s="24"/>
       <c r="V36" s="25"/>
-      <c r="W36" s="26" t="n">
-        <f aca="false">B36-SUM(C36:V36)</f>
+      <c r="W36" s="26">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="X36" s="21" t="str">
-        <f aca="false">IFERROR(1-(W36/B36),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="37" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="27" t="s">
         <v>40</v>
       </c>
@@ -3627,219 +4043,218 @@
       <c r="T37" s="30"/>
       <c r="U37" s="29"/>
       <c r="V37" s="30"/>
-      <c r="W37" s="31" t="n">
-        <f aca="false">B37-SUM(C37:V37)</f>
+      <c r="W37" s="31">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="X37" s="32" t="str">
-        <f aca="false">IFERROR(1-(W37/B37),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" spans="1:24" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A38" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="B38" s="34" t="n">
-        <f aca="false">SUM(B8:B37)</f>
+      <c r="B38" s="34">
+        <f>SUM(B8:B37)</f>
         <v>69</v>
       </c>
-      <c r="C38" s="35" t="n">
-        <f aca="false">IFERROR(IF(B38-SUM(C8:C37)=B38,NA(),B38-SUM(C8:C37)),NA())</f>
-        <v>68</v>
-      </c>
-      <c r="D38" s="35" t="e">
-        <f aca="false">IFERROR(IF(C38-SUM(D8:D37)=C38,NA(),C38-SUM(D8:D37)),NA())</f>
+      <c r="C38" s="35">
+        <f t="shared" ref="C38:V38" si="2">IFERROR(IF(B38-SUM(C8:C37)=B38,NA(),B38-SUM(C8:C37)),NA())</f>
+        <v>66</v>
+      </c>
+      <c r="D38" s="35">
+        <f t="shared" si="2"/>
+        <v>65</v>
+      </c>
+      <c r="E38" s="35" t="e">
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
-      <c r="E38" s="35" t="e">
-        <f aca="false">IFERROR(IF(D38-SUM(E8:E37)=D38,NA(),D38-SUM(E8:E37)),NA())</f>
+      <c r="F38" s="35" t="e">
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
-      <c r="F38" s="35" t="e">
-        <f aca="false">IFERROR(IF(E38-SUM(F8:F37)=E38,NA(),E38-SUM(F8:F37)),NA())</f>
+      <c r="G38" s="35" t="e">
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
-      <c r="G38" s="35" t="e">
-        <f aca="false">IFERROR(IF(F38-SUM(G8:G37)=F38,NA(),F38-SUM(G8:G37)),NA())</f>
+      <c r="H38" s="35" t="e">
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
-      <c r="H38" s="35" t="e">
-        <f aca="false">IFERROR(IF(G38-SUM(H8:H37)=G38,NA(),G38-SUM(H8:H37)),NA())</f>
+      <c r="I38" s="35" t="e">
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
-      <c r="I38" s="35" t="e">
-        <f aca="false">IFERROR(IF(H38-SUM(I8:I37)=H38,NA(),H38-SUM(I8:I37)),NA())</f>
+      <c r="J38" s="35" t="e">
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
-      <c r="J38" s="35" t="e">
-        <f aca="false">IFERROR(IF(I38-SUM(J8:J37)=I38,NA(),I38-SUM(J8:J37)),NA())</f>
+      <c r="K38" s="35" t="e">
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
-      <c r="K38" s="35" t="e">
-        <f aca="false">IFERROR(IF(J38-SUM(K8:K37)=J38,NA(),J38-SUM(K8:K37)),NA())</f>
+      <c r="L38" s="35" t="e">
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
-      <c r="L38" s="35" t="e">
-        <f aca="false">IFERROR(IF(K38-SUM(L8:L37)=K38,NA(),K38-SUM(L8:L37)),NA())</f>
+      <c r="M38" s="35" t="e">
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
-      <c r="M38" s="35" t="e">
-        <f aca="false">IFERROR(IF(L38-SUM(M8:M37)=L38,NA(),L38-SUM(M8:M37)),NA())</f>
+      <c r="N38" s="35" t="e">
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
-      <c r="N38" s="35" t="e">
-        <f aca="false">IFERROR(IF(M38-SUM(N8:N37)=M38,NA(),M38-SUM(N8:N37)),NA())</f>
+      <c r="O38" s="35" t="e">
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
-      <c r="O38" s="35" t="e">
-        <f aca="false">IFERROR(IF(N38-SUM(O8:O37)=N38,NA(),N38-SUM(O8:O37)),NA())</f>
+      <c r="P38" s="35" t="e">
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
-      <c r="P38" s="35" t="e">
-        <f aca="false">IFERROR(IF(O38-SUM(P8:P37)=O38,NA(),O38-SUM(P8:P37)),NA())</f>
+      <c r="Q38" s="35" t="e">
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
-      <c r="Q38" s="35" t="e">
-        <f aca="false">IFERROR(IF(P38-SUM(Q8:Q37)=P38,NA(),P38-SUM(Q8:Q37)),NA())</f>
+      <c r="R38" s="35" t="e">
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
-      <c r="R38" s="35" t="e">
-        <f aca="false">IFERROR(IF(Q38-SUM(R8:R37)=Q38,NA(),Q38-SUM(R8:R37)),NA())</f>
+      <c r="S38" s="35" t="e">
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
-      <c r="S38" s="35" t="e">
-        <f aca="false">IFERROR(IF(R38-SUM(S8:S37)=R38,NA(),R38-SUM(S8:S37)),NA())</f>
+      <c r="T38" s="35" t="e">
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
-      <c r="T38" s="35" t="e">
-        <f aca="false">IFERROR(IF(S38-SUM(T8:T37)=S38,NA(),S38-SUM(T8:T37)),NA())</f>
+      <c r="U38" s="35" t="e">
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
-      <c r="U38" s="35" t="e">
-        <f aca="false">IFERROR(IF(T38-SUM(U8:U37)=T38,NA(),T38-SUM(U8:U37)),NA())</f>
+      <c r="V38" s="35" t="e">
+        <f t="shared" si="2"/>
         <v>#N/A</v>
       </c>
-      <c r="V38" s="35" t="e">
-        <f aca="false">IFERROR(IF(U38-SUM(V8:V37)=U38,NA(),U38-SUM(V8:V37)),NA())</f>
-        <v>#N/A</v>
-      </c>
-      <c r="W38" s="36" t="n">
-        <f aca="false">SUM(W8:W37)</f>
-        <v>61</v>
-      </c>
-      <c r="X38" s="37" t="n">
-        <f aca="false">IFERROR(1-(W38/B38),"")</f>
-        <v>0.115942028985507</v>
+      <c r="W38" s="36">
+        <f>SUM(W8:W37)</f>
+        <v>55</v>
+      </c>
+      <c r="X38" s="37">
+        <f t="shared" si="1"/>
+        <v>0.20289855072463769</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" spans="1:24" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A39" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="B39" s="39" t="n">
-        <f aca="false">SUM(B8:B37)</f>
+      <c r="B39" s="39">
+        <f>SUM(B8:B37)</f>
         <v>69</v>
       </c>
-      <c r="C39" s="40" t="n">
-        <f aca="false">IFERROR((IF(B39-($B$38/$G$4) &lt; 0,"-", B39-($B$38/$G$4))),IFERROR(B39-($B$38/20),"-"))</f>
+      <c r="C39" s="40">
+        <f t="shared" ref="C39:V39" si="3">IFERROR((IF(B39-($B$38/$G$4) &lt; 0,"-", B39-($B$38/$G$4))),IFERROR(B39-($B$38/20),"-"))</f>
         <v>65.55</v>
       </c>
-      <c r="D39" s="40" t="n">
-        <f aca="false">IFERROR((IF(C39-($B$38/$G$4) &lt; 0,"-", C39-($B$38/$G$4))),IFERROR(C39-($B$38/20),"-"))</f>
-        <v>62.1</v>
-      </c>
-      <c r="E39" s="40" t="n">
-        <f aca="false">IFERROR((IF(D39-($B$38/$G$4) &lt; 0,"-", D39-($B$38/$G$4))),IFERROR(D39-($B$38/20),"-"))</f>
-        <v>58.65</v>
-      </c>
-      <c r="F39" s="40" t="n">
-        <f aca="false">IFERROR((IF(E39-($B$38/$G$4) &lt; 0,"-", E39-($B$38/$G$4))),IFERROR(E39-($B$38/20),"-"))</f>
-        <v>55.2</v>
-      </c>
-      <c r="G39" s="40" t="n">
-        <f aca="false">IFERROR((IF(F39-($B$38/$G$4) &lt; 0,"-", F39-($B$38/$G$4))),IFERROR(F39-($B$38/20),"-"))</f>
-        <v>51.75</v>
-      </c>
-      <c r="H39" s="40" t="n">
-        <f aca="false">IFERROR((IF(G39-($B$38/$G$4) &lt; 0,"-", G39-($B$38/$G$4))),IFERROR(G39-($B$38/20),"-"))</f>
-        <v>48.3</v>
-      </c>
-      <c r="I39" s="40" t="n">
-        <f aca="false">IFERROR((IF(H39-($B$38/$G$4) &lt; 0,"-", H39-($B$38/$G$4))),IFERROR(H39-($B$38/20),"-"))</f>
-        <v>44.85</v>
-      </c>
-      <c r="J39" s="40" t="n">
-        <f aca="false">IFERROR((IF(I39-($B$38/$G$4) &lt; 0,"-", I39-($B$38/$G$4))),IFERROR(I39-($B$38/20),"-"))</f>
-        <v>41.4</v>
-      </c>
-      <c r="K39" s="40" t="n">
-        <f aca="false">IFERROR((IF(J39-($B$38/$G$4) &lt; 0,"-", J39-($B$38/$G$4))),IFERROR(J39-($B$38/20),"-"))</f>
-        <v>37.95</v>
-      </c>
-      <c r="L39" s="40" t="n">
-        <f aca="false">IFERROR((IF(K39-($B$38/$G$4) &lt; 0,"-", K39-($B$38/$G$4))),IFERROR(K39-($B$38/20),"-"))</f>
-        <v>34.5</v>
-      </c>
-      <c r="M39" s="40" t="n">
-        <f aca="false">IFERROR((IF(L39-($B$38/$G$4) &lt; 0,"-", L39-($B$38/$G$4))),IFERROR(L39-($B$38/20),"-"))</f>
-        <v>31.05</v>
-      </c>
-      <c r="N39" s="40" t="n">
-        <f aca="false">IFERROR((IF(M39-($B$38/$G$4) &lt; 0,"-", M39-($B$38/$G$4))),IFERROR(M39-($B$38/20),"-"))</f>
-        <v>27.6</v>
-      </c>
-      <c r="O39" s="40" t="n">
-        <f aca="false">IFERROR((IF(N39-($B$38/$G$4) &lt; 0,"-", N39-($B$38/$G$4))),IFERROR(N39-($B$38/20),"-"))</f>
-        <v>24.15</v>
-      </c>
-      <c r="P39" s="40" t="n">
-        <f aca="false">IFERROR((IF(O39-($B$38/$G$4) &lt; 0,"-", O39-($B$38/$G$4))),IFERROR(O39-($B$38/20),"-"))</f>
-        <v>20.7</v>
-      </c>
-      <c r="Q39" s="40" t="n">
-        <f aca="false">IFERROR((IF(P39-($B$38/$G$4) &lt; 0,"-", P39-($B$38/$G$4))),IFERROR(P39-($B$38/20),"-"))</f>
-        <v>17.25</v>
-      </c>
-      <c r="R39" s="40" t="n">
-        <f aca="false">IFERROR((IF(Q39-($B$38/$G$4) &lt; 0,"-", Q39-($B$38/$G$4))),IFERROR(Q39-($B$38/20),"-"))</f>
-        <v>13.8</v>
-      </c>
-      <c r="S39" s="40" t="n">
-        <f aca="false">IFERROR((IF(R39-($B$38/$G$4) &lt; 0,"-", R39-($B$38/$G$4))),IFERROR(R39-($B$38/20),"-"))</f>
-        <v>10.35</v>
-      </c>
-      <c r="T39" s="40" t="n">
-        <f aca="false">IFERROR((IF(S39-($B$38/$G$4) &lt; 0,"-", S39-($B$38/$G$4))),IFERROR(S39-($B$38/20),"-"))</f>
-        <v>6.89999999999998</v>
-      </c>
-      <c r="U39" s="40" t="n">
-        <f aca="false">IFERROR((IF(T39-($B$38/$G$4) &lt; 0,"-", T39-($B$38/$G$4))),IFERROR(T39-($B$38/20),"-"))</f>
-        <v>3.44999999999998</v>
-      </c>
-      <c r="V39" s="40" t="n">
-        <f aca="false">IFERROR((IF(U39-($B$38/$G$4) &lt; 0,"-", U39-($B$38/$G$4))),IFERROR(U39-($B$38/20),"-"))</f>
-        <v>-2.39808173319034E-014</v>
+      <c r="D39" s="40">
+        <f t="shared" si="3"/>
+        <v>62.099999999999994</v>
+      </c>
+      <c r="E39" s="40">
+        <f t="shared" si="3"/>
+        <v>58.649999999999991</v>
+      </c>
+      <c r="F39" s="40">
+        <f t="shared" si="3"/>
+        <v>55.199999999999989</v>
+      </c>
+      <c r="G39" s="40">
+        <f t="shared" si="3"/>
+        <v>51.749999999999986</v>
+      </c>
+      <c r="H39" s="40">
+        <f t="shared" si="3"/>
+        <v>48.299999999999983</v>
+      </c>
+      <c r="I39" s="40">
+        <f t="shared" si="3"/>
+        <v>44.84999999999998</v>
+      </c>
+      <c r="J39" s="40">
+        <f t="shared" si="3"/>
+        <v>41.399999999999977</v>
+      </c>
+      <c r="K39" s="40">
+        <f t="shared" si="3"/>
+        <v>37.949999999999974</v>
+      </c>
+      <c r="L39" s="40">
+        <f t="shared" si="3"/>
+        <v>34.499999999999972</v>
+      </c>
+      <c r="M39" s="40">
+        <f t="shared" si="3"/>
+        <v>31.049999999999972</v>
+      </c>
+      <c r="N39" s="40">
+        <f t="shared" si="3"/>
+        <v>27.599999999999973</v>
+      </c>
+      <c r="O39" s="40">
+        <f t="shared" si="3"/>
+        <v>24.149999999999974</v>
+      </c>
+      <c r="P39" s="40">
+        <f t="shared" si="3"/>
+        <v>20.699999999999974</v>
+      </c>
+      <c r="Q39" s="40">
+        <f t="shared" si="3"/>
+        <v>17.249999999999975</v>
+      </c>
+      <c r="R39" s="40">
+        <f t="shared" si="3"/>
+        <v>13.799999999999976</v>
+      </c>
+      <c r="S39" s="40">
+        <f t="shared" si="3"/>
+        <v>10.349999999999977</v>
+      </c>
+      <c r="T39" s="40">
+        <f t="shared" si="3"/>
+        <v>6.8999999999999764</v>
+      </c>
+      <c r="U39" s="40">
+        <f t="shared" si="3"/>
+        <v>3.4499999999999762</v>
+      </c>
+      <c r="V39" s="40">
+        <f t="shared" si="3"/>
+        <v>-2.3980817331903381E-14</v>
       </c>
       <c r="W39" s="41"/>
       <c r="X39" s="42"/>
     </row>
-    <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:V6"/>
+    <mergeCell ref="W6:X6"/>
     <mergeCell ref="A1:B2"/>
     <mergeCell ref="C2:F2"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="C3:F3"/>
     <mergeCell ref="H3:I3"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:V6"/>
-    <mergeCell ref="W6:X6"/>
   </mergeCells>
   <conditionalFormatting sqref="X8:X38">
     <cfRule type="dataBar" priority="2">
-      <dataBar showValue="1" minLength="10" maxLength="90">
+      <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
         <color rgb="FF63C384"/>
@@ -3851,21 +4266,16 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{113B4CE2-8C96-4116-8A18-E052C995704E}">
-            <x14:dataBar minLength="10" maxLength="90" axisPosition="automatic" gradient="false">
+            <x14:dataBar gradient="0">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>
               </x14:cfvo>
@@ -3885,25 +4295,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T37" activeCellId="0" sqref="T37"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T37" sqref="T37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>